<commit_message>
add not accurate timer wheel for better performance
Signed-off-by: Hanoh Haim <hhaim@cisco.com>
</commit_message>
<xml_diff>
--- a/doc/visio_drawings/tw.xlsx
+++ b/doc/visio_drawings/tw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="705" windowWidth="12420" windowHeight="12720"/>
+    <workbookView xWindow="180" yWindow="-135" windowWidth="17490" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>active-flows</t>
   </si>
@@ -32,6 +32,9 @@
   <si>
     <t>TW2</t>
   </si>
+  <si>
+    <t>TW3  v2.14</t>
+  </si>
 </sst>
 </file>
 
@@ -39,7 +42,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -95,11 +98,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -108,17 +112,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -573,11 +579,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="245212672"/>
-        <c:axId val="245214208"/>
+        <c:axId val="234522880"/>
+        <c:axId val="236196608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="245212672"/>
+        <c:axId val="234522880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +612,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245214208"/>
+        <c:crossAx val="236196608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245214208"/>
+        <c:axId val="236196608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +650,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245212672"/>
+        <c:crossAx val="234522880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1109,11 +1115,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="247186944"/>
-        <c:axId val="247188480"/>
+        <c:axId val="244794112"/>
+        <c:axId val="244796032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="247186944"/>
+        <c:axId val="244794112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1153,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247188480"/>
+        <c:crossAx val="244796032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1155,7 +1161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247188480"/>
+        <c:axId val="244796032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1196,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247186944"/>
+        <c:crossAx val="244794112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1655,11 +1661,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="251461632"/>
-        <c:axId val="251463552"/>
+        <c:axId val="247157888"/>
+        <c:axId val="250404864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="251461632"/>
+        <c:axId val="247157888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1681,14 +1687,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251463552"/>
+        <c:crossAx val="250404864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1696,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251463552"/>
+        <c:axId val="250404864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1743,14 +1748,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251461632"/>
+        <c:crossAx val="247157888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2150,7 +2154,7 @@
   <dimension ref="A3:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R98" sqref="R98"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +2165,7 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2177,8 +2181,11 @@
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100</v>
       </c>
@@ -2194,8 +2201,15 @@
       <c r="E4" s="4">
         <v>5207908.585331942</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="4">
+        <v>5333996.4463397292</v>
+      </c>
+      <c r="G4" s="7">
+        <f>F4/C4</f>
+        <v>1.0332514044840861</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>285</v>
       </c>
@@ -2211,8 +2225,15 @@
       <c r="E5" s="4">
         <v>5193260.0554785011</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="4">
+        <v>5260815.1260504201</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G14" si="0">F5/C5</f>
+        <v>1.0190754104181703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>866</v>
       </c>
@@ -2228,8 +2249,15 @@
       <c r="E6" s="4">
         <v>5169301.9323671507</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="4">
+        <v>5137760.4237867398</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0261442544781438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2667</v>
       </c>
@@ -2245,8 +2273,15 @@
       <c r="E7" s="4">
         <v>5141350.2747252742</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="4">
+        <v>5137512.8468653644</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.035654236748432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>8240</v>
       </c>
@@ -2262,8 +2297,15 @@
       <c r="E8" s="4">
         <v>5060864.5727794673</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="4">
+        <v>5040941.8487394964</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0203049443563623</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>25452</v>
       </c>
@@ -2279,8 +2321,15 @@
       <c r="E9" s="4">
         <v>4814287.636130685</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="4">
+        <v>4883432.8018223243</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0163316135519687</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>78740</v>
       </c>
@@ -2296,8 +2345,15 @@
       <c r="E10" s="4">
         <v>4507848.5407066057</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="4">
+        <v>4558750.7598784193</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0113706136806473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>243449</v>
       </c>
@@ -2313,8 +2369,15 @@
       <c r="E11" s="4">
         <v>4441207.9027355621</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="4">
+        <v>3762094.4862155388</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0167766562080403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>752862</v>
       </c>
@@ -2330,8 +2393,15 @@
       <c r="E12" s="4">
         <v>4346235.2062163781</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="4">
+        <v>3927404.9803407602</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4083548466537159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2328217</v>
       </c>
@@ -2347,8 +2417,15 @@
       <c r="E13" s="4">
         <v>4452171.0048426148</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="4">
+        <v>3796069.785082174</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>1.272617606558321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7199980</v>
       </c>
@@ -2363,6 +2440,13 @@
       </c>
       <c r="E14" s="4">
         <v>4738613.5406543566</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3431939.9220362306</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.13133266606834</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2444,19 +2528,19 @@
         <v>5193260.0554785011</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" ref="F45:F54" si="0">B45/B45</f>
+        <f t="shared" ref="F45:F54" si="1">B45/B45</f>
         <v>1</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" ref="G45:G54" si="1">C45/B45</f>
+        <f t="shared" ref="G45:G54" si="2">C45/B45</f>
         <v>1.125</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" ref="H45:H54" si="2">D45/B45</f>
+        <f t="shared" ref="H45:H54" si="3">D45/B45</f>
         <v>1.1215327424052757</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" ref="I45:I54" si="3">E45/B45</f>
+        <f t="shared" ref="I45:I54" si="4">E45/B45</f>
         <v>1.1317379403371208</v>
       </c>
     </row>
@@ -2477,19 +2561,19 @@
         <v>5169301.9323671507</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0911167830685753</v>
       </c>
       <c r="H46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0945088655230011</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1265168813848008</v>
       </c>
     </row>
@@ -2510,19 +2594,19 @@
         <v>5141350.2747252742</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2750792082364948</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2777381552801781</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3215275528342514</v>
       </c>
     </row>
@@ -2543,19 +2627,19 @@
         <v>5060864.5727794673</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6426304140444206</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6673082190014443</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6826077281964058</v>
       </c>
     </row>
@@ -2576,19 +2660,19 @@
         <v>4814287.636130685</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4914607672549502</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4704464153732442</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4962972928085034</v>
       </c>
     </row>
@@ -2609,19 +2693,19 @@
         <v>4507848.5407066057</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0275547772713405</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9906584801893898</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0277125718720082</v>
       </c>
     </row>
@@ -2642,19 +2726,19 @@
         <v>4441207.9027355621</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5229284435986159</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5096950256410258</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8280011727659571</v>
       </c>
     </row>
@@ -2675,19 +2759,19 @@
         <v>4346235.2062163781</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3195879157251909</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7442996419243986</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0566384995815898</v>
       </c>
     </row>
@@ -2708,19 +2792,19 @@
         <v>4452171.0048426148</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5326054311396471</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9853112972972975</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2875254622881358</v>
       </c>
     </row>
@@ -2741,19 +2825,19 @@
         <v>4738613.5406543566</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.63082969088</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.0094209780869563</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.547478639455782</v>
       </c>
     </row>
@@ -2813,15 +2897,15 @@
         <v>308.36385641025635</v>
       </c>
       <c r="G86" s="6">
-        <f t="shared" ref="G86:G96" si="4">C86*$D$83</f>
+        <f t="shared" ref="G86:G96" si="5">C86*$D$83</f>
         <v>346.90933846153843</v>
       </c>
       <c r="H86" s="6">
-        <f t="shared" ref="H86:H96" si="5">D86*$D$83</f>
+        <f t="shared" ref="H86:H96" si="6">D86*$D$83</f>
         <v>350.75980145985397</v>
       </c>
       <c r="I86" s="6">
-        <f t="shared" ref="I86:I96" si="6">E86*$D$83</f>
+        <f t="shared" ref="I86:I96" si="7">E86*$D$83</f>
         <v>349.97145693430645</v>
       </c>
     </row>
@@ -2842,19 +2926,19 @@
         <v>5193260.0554785011</v>
       </c>
       <c r="F87" s="6">
-        <f t="shared" ref="F87:F96" si="7">B87*$D$83</f>
+        <f t="shared" ref="F87:F96" si="8">B87*$D$83</f>
         <v>308.36385641025635</v>
       </c>
       <c r="G87" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>346.90933846153843</v>
       </c>
       <c r="H87" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>345.84016153846147</v>
       </c>
       <c r="I87" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>348.98707572815522</v>
       </c>
     </row>
@@ -2875,19 +2959,19 @@
         <v>5169301.9323671507</v>
       </c>
       <c r="F88" s="6">
+        <f t="shared" si="8"/>
+        <v>308.36385641025635</v>
+      </c>
+      <c r="G88" s="6">
+        <f t="shared" si="5"/>
+        <v>336.46097902097898</v>
+      </c>
+      <c r="H88" s="6">
+        <f t="shared" si="6"/>
+        <v>337.50697464788732</v>
+      </c>
+      <c r="I88" s="6">
         <f t="shared" si="7"/>
-        <v>308.36385641025635</v>
-      </c>
-      <c r="G88" s="6">
-        <f t="shared" si="4"/>
-        <v>336.46097902097898</v>
-      </c>
-      <c r="H88" s="6">
-        <f t="shared" si="5"/>
-        <v>337.50697464788732</v>
-      </c>
-      <c r="I88" s="6">
-        <f t="shared" si="6"/>
         <v>347.37708985507248</v>
       </c>
     </row>
@@ -2908,19 +2992,19 @@
         <v>5141350.2747252742</v>
       </c>
       <c r="F89" s="6">
+        <f t="shared" si="8"/>
+        <v>261.43892173913042</v>
+      </c>
+      <c r="G89" s="6">
+        <f t="shared" si="5"/>
+        <v>333.35533333333331</v>
+      </c>
+      <c r="H89" s="6">
+        <f t="shared" si="6"/>
+        <v>334.05048558139532</v>
+      </c>
+      <c r="I89" s="6">
         <f t="shared" si="7"/>
-        <v>261.43892173913042</v>
-      </c>
-      <c r="G89" s="6">
-        <f t="shared" si="4"/>
-        <v>333.35533333333331</v>
-      </c>
-      <c r="H89" s="6">
-        <f t="shared" si="5"/>
-        <v>334.05048558139532</v>
-      </c>
-      <c r="I89" s="6">
-        <f t="shared" si="6"/>
         <v>345.49873846153838</v>
       </c>
     </row>
@@ -2941,19 +3025,19 @@
         <v>5060864.5727794673</v>
       </c>
       <c r="F90" s="6">
+        <f t="shared" si="8"/>
+        <v>202.1208470588235</v>
+      </c>
+      <c r="G90" s="6">
+        <f t="shared" si="5"/>
+        <v>332.00985069124425</v>
+      </c>
+      <c r="H90" s="6">
+        <f t="shared" si="6"/>
+        <v>336.99774953271032</v>
+      </c>
+      <c r="I90" s="6">
         <f t="shared" si="7"/>
-        <v>202.1208470588235</v>
-      </c>
-      <c r="G90" s="6">
-        <f t="shared" si="4"/>
-        <v>332.00985069124425</v>
-      </c>
-      <c r="H90" s="6">
-        <f t="shared" si="5"/>
-        <v>336.99774953271032</v>
-      </c>
-      <c r="I90" s="6">
-        <f t="shared" si="6"/>
         <v>340.09009929078019</v>
       </c>
     </row>
@@ -2974,19 +3058,19 @@
         <v>4814287.636130685</v>
       </c>
       <c r="F91" s="6">
+        <f t="shared" si="8"/>
+        <v>129.6</v>
+      </c>
+      <c r="G91" s="6">
+        <f t="shared" si="5"/>
+        <v>322.89331543624155</v>
+      </c>
+      <c r="H91" s="6">
+        <f t="shared" si="6"/>
+        <v>320.16985543237246</v>
+      </c>
+      <c r="I91" s="6">
         <f t="shared" si="7"/>
-        <v>129.6</v>
-      </c>
-      <c r="G91" s="6">
-        <f t="shared" si="4"/>
-        <v>322.89331543624155</v>
-      </c>
-      <c r="H91" s="6">
-        <f t="shared" si="5"/>
-        <v>320.16985543237246</v>
-      </c>
-      <c r="I91" s="6">
-        <f t="shared" si="6"/>
         <v>323.520129147982</v>
       </c>
     </row>
@@ -3007,19 +3091,19 @@
         <v>4507848.5407066057</v>
       </c>
       <c r="F92" s="6">
+        <f t="shared" si="8"/>
+        <v>149.39366956521738</v>
+      </c>
+      <c r="G92" s="6">
+        <f t="shared" si="5"/>
+        <v>302.9038484210526</v>
+      </c>
+      <c r="H92" s="6">
+        <f t="shared" si="6"/>
+        <v>297.39177520661156</v>
+      </c>
+      <c r="I92" s="6">
         <f t="shared" si="7"/>
-        <v>149.39366956521738</v>
-      </c>
-      <c r="G92" s="6">
-        <f t="shared" si="4"/>
-        <v>302.9038484210526</v>
-      </c>
-      <c r="H92" s="6">
-        <f t="shared" si="5"/>
-        <v>297.39177520661156</v>
-      </c>
-      <c r="I92" s="6">
-        <f t="shared" si="6"/>
         <v>302.92742193548389</v>
       </c>
     </row>
@@ -3040,19 +3124,19 @@
         <v>4441207.9027355621</v>
       </c>
       <c r="F93" s="6">
+        <f t="shared" si="8"/>
+        <v>163.26530612244898</v>
+      </c>
+      <c r="G93" s="6">
+        <f t="shared" si="5"/>
+        <v>248.64137854671282</v>
+      </c>
+      <c r="H93" s="6">
+        <f t="shared" si="6"/>
+        <v>246.48082051282051</v>
+      </c>
+      <c r="I93" s="6">
         <f t="shared" si="7"/>
-        <v>163.26530612244898</v>
-      </c>
-      <c r="G93" s="6">
-        <f t="shared" si="4"/>
-        <v>248.64137854671282</v>
-      </c>
-      <c r="H93" s="6">
-        <f t="shared" si="5"/>
-        <v>246.48082051282051</v>
-      </c>
-      <c r="I93" s="6">
-        <f t="shared" si="6"/>
         <v>298.44917106382974</v>
       </c>
     </row>
@@ -3073,19 +3157,19 @@
         <v>4346235.2062163781</v>
       </c>
       <c r="F94" s="6">
+        <f t="shared" si="8"/>
+        <v>142.01183431952663</v>
+      </c>
+      <c r="G94" s="6">
+        <f t="shared" si="5"/>
+        <v>187.39710045801525</v>
+      </c>
+      <c r="H94" s="6">
+        <f t="shared" si="6"/>
+        <v>247.71119175257729</v>
+      </c>
+      <c r="I94" s="6">
         <f t="shared" si="7"/>
-        <v>142.01183431952663</v>
-      </c>
-      <c r="G94" s="6">
-        <f t="shared" si="4"/>
-        <v>187.39710045801525</v>
-      </c>
-      <c r="H94" s="6">
-        <f t="shared" si="5"/>
-        <v>247.71119175257729</v>
-      </c>
-      <c r="I94" s="6">
-        <f t="shared" si="6"/>
         <v>292.06700585774058</v>
       </c>
     </row>
@@ -3106,19 +3190,19 @@
         <v>4452171.0048426148</v>
       </c>
       <c r="F95" s="6">
+        <f t="shared" si="8"/>
+        <v>130.79019073569481</v>
+      </c>
+      <c r="G95" s="6">
+        <f t="shared" si="5"/>
+        <v>200.4497566613162</v>
+      </c>
+      <c r="H95" s="6">
+        <f t="shared" si="6"/>
+        <v>259.65924324324322</v>
+      </c>
+      <c r="I95" s="6">
         <f t="shared" si="7"/>
-        <v>130.79019073569481</v>
-      </c>
-      <c r="G95" s="6">
-        <f t="shared" si="4"/>
-        <v>200.4497566613162</v>
-      </c>
-      <c r="H95" s="6">
-        <f t="shared" si="5"/>
-        <v>259.65924324324322</v>
-      </c>
-      <c r="I95" s="6">
-        <f t="shared" si="6"/>
         <v>299.1858915254237</v>
       </c>
     </row>
@@ -3139,19 +3223,19 @@
         <v>4738613.5406543566</v>
       </c>
       <c r="F96" s="6">
+        <f t="shared" si="8"/>
+        <v>125</v>
+      </c>
+      <c r="G96" s="6">
+        <f t="shared" si="5"/>
+        <v>203.85371136000001</v>
+      </c>
+      <c r="H96" s="6">
+        <f t="shared" si="6"/>
+        <v>251.17762226086955</v>
+      </c>
+      <c r="I96" s="6">
         <f t="shared" si="7"/>
-        <v>125</v>
-      </c>
-      <c r="G96" s="6">
-        <f t="shared" si="4"/>
-        <v>203.85371136000001</v>
-      </c>
-      <c r="H96" s="6">
-        <f t="shared" si="5"/>
-        <v>251.17762226086955</v>
-      </c>
-      <c r="I96" s="6">
-        <f t="shared" si="6"/>
         <v>318.43482993197273</v>
       </c>
     </row>

</xml_diff>